<commit_message>
fix: use html2pdf library instead of weasyprint
</commit_message>
<xml_diff>
--- a/media/legalizacion_1.xlsx
+++ b/media/legalizacion_1.xlsx
@@ -553,7 +553,7 @@
         </is>
       </c>
       <c r="B6" s="7" t="n">
-        <v>45047</v>
+        <v>45411</v>
       </c>
       <c r="I6" s="5" t="n"/>
       <c r="AE6" s="3" t="n"/>
@@ -567,7 +567,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I7" s="5" t="n"/>
@@ -582,7 +582,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1234567890</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E8" s="6" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I8" s="5" t="n"/>
@@ -607,7 +607,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Departamento de Ventas</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I9" s="5" t="n"/>
@@ -623,7 +623,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I11" s="5" t="n"/>
@@ -635,7 +635,7 @@
         </is>
       </c>
       <c r="B12" s="7" t="n">
-        <v>45031</v>
+        <v>45411</v>
       </c>
       <c r="E12" s="6" t="inlineStr">
         <is>
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="F12" s="7" t="n">
-        <v>45036</v>
+        <v>45411</v>
       </c>
       <c r="I12" s="5" t="n"/>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Reunión de negocios</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I13" s="5" t="n"/>
@@ -736,31 +736,31 @@
     <row r="20">
       <c r="A20" s="10" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B20" s="10" t="inlineStr">
         <is>
-          <t>12345</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>Transportes S.A.</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>123456789</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E20" s="10" t="inlineStr">
         <is>
-          <t>Taxis y buses</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F20" s="10" t="n">
-        <v>100000</v>
+        <v>1</v>
       </c>
       <c r="G20" s="10" t="n"/>
       <c r="H20" s="10" t="n"/>
@@ -911,7 +911,7 @@
       <c r="D32" s="10" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n">
-        <v>1000000</v>
+        <v>1</v>
       </c>
       <c r="G32" s="10" t="n">
         <v>0</v>
@@ -998,12 +998,12 @@
     <row r="40">
       <c r="A40" s="12" t="inlineStr">
         <is>
-          <t>Pedro Gómez</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E40" s="12" t="inlineStr">
         <is>
-          <t>María Rodríguez</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I40" s="5" t="n"/>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Banco de Bogotá</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D45" s="6" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1234567890</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I46" s="5" t="n"/>

</xml_diff>